<commit_message>
update file Visualization và 1 đống file xlsx :angel:
File Visualization nằm trong folder Source/beta/experiments.
</commit_message>
<xml_diff>
--- a/Result/Data Preprocessing.xlsx
+++ b/Result/Data Preprocessing.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/becdff2ddfbd42e8/Documents/GitHub/PythonScrapJob/Result/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tam\OneDrive\Documents\GitHub\PythonScrapJob\Result\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="105" windowWidth="14130" windowHeight="8010"/>
+    <workbookView xWindow="3090" yWindow="105" windowWidth="14130" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>Website</t>
   </si>
@@ -17019,8 +17019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84:M89"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17153,7 +17153,9 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="11" t="s">
+        <v>0</v>
+      </c>
       <c r="B17" s="10" t="s">
         <v>23</v>
       </c>
@@ -17379,7 +17381,7 @@
       <c r="P52"/>
       <c r="Q52"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>39</v>
       </c>

</xml_diff>